<commit_message>
En la simulacion falta que retome el valor actual donde se quedo quieta la maquina y que los demas esperen a que llegue
</commit_message>
<xml_diff>
--- a/AlgoritmoSimulacion.xlsx
+++ b/AlgoritmoSimulacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\Desktop\Carlos\Universidad\2do_semestre_2021\IPC 2\Laboratorio\Proyecto 2\IPC2_Proyecto2_201905515\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1219ACA-3102-42A3-89E0-09DB2B5B445F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B282CBF0-70D4-43E6-A1E2-1B4BE821EE40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15480" yWindow="-120" windowWidth="15600" windowHeight="11040" xr2:uid="{50457206-07E3-4C7A-B93E-7578EA5904F6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1426" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="124">
   <si>
     <t>Lineas</t>
   </si>
@@ -406,7 +406,7 @@
     <t>true</t>
   </si>
   <si>
-    <t>ComponenteA</t>
+    <t>LineaOcupada</t>
   </si>
 </sst>
 </file>
@@ -3298,8 +3298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8616836-1540-4FB5-9159-4EB3A710534F}">
   <dimension ref="A2:V68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4017,8 +4017,8 @@
       <c r="C44">
         <v>9</v>
       </c>
-      <c r="D44">
-        <v>0</v>
+      <c r="D44" t="s">
+        <v>24</v>
       </c>
       <c r="E44" t="s">
         <v>98</v>
@@ -4027,7 +4027,7 @@
         <v>122</v>
       </c>
       <c r="G44" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>115</v>

</xml_diff>